<commit_message>
Added graphs for credits study
</commit_message>
<xml_diff>
--- a/src/dataset.xlsx
+++ b/src/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emili\OneDrive\Escritorio\Universidad\4Carrera\AcademicData\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4E72B5-B546-4117-8CB3-D43446C7C6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C1C150-0D81-4C43-8C2D-283DE415592C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{82361F5A-4340-435D-A49C-2C3E84564897}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82361F5A-4340-435D-A49C-2C3E84564897}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="73">
   <si>
     <t>Year</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Calculus</t>
   </si>
   <si>
-    <t>Fisics</t>
-  </si>
-  <si>
     <t>Electronics</t>
   </si>
   <si>
@@ -227,15 +224,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>BF</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
     <t>TFG</t>
   </si>
   <si>
@@ -249,14 +237,40 @@
   </si>
   <si>
     <t>Programming Languages</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>Basic Formation</t>
+  </si>
+  <si>
+    <t>Mandatory</t>
+  </si>
+  <si>
+    <t>Optative (Mention)</t>
+  </si>
+  <si>
+    <t>Optative</t>
+  </si>
+  <si>
+    <t>Optative (Internship)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -284,11 +298,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,21 +641,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B16DEB-C3AC-4914-94E8-AA9D57CD36CC}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>68</v>
+      <c r="A1" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -646,22 +666,22 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -672,22 +692,22 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2">
         <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -695,28 +715,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3">
         <v>6</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -724,28 +744,28 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4">
         <v>6</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -753,28 +773,28 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5">
         <v>6</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -782,28 +802,28 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G6">
         <v>6</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -811,7 +831,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -820,19 +840,19 @@
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7">
         <v>6</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I7">
         <v>2</v>
@@ -840,28 +860,28 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G8">
         <v>6</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -869,28 +889,28 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9">
         <v>6</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I9">
         <v>2</v>
@@ -898,28 +918,28 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G10">
         <v>6</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I10">
         <v>2</v>
@@ -927,7 +947,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -936,19 +956,19 @@
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G11">
         <v>6</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I11">
         <v>2</v>
@@ -956,7 +976,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1">
         <v>2</v>
@@ -965,19 +985,19 @@
         <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12">
         <v>6</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -985,28 +1005,28 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1">
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G13">
         <v>6</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -1014,7 +1034,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1">
         <v>2</v>
@@ -1023,19 +1043,19 @@
         <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G14">
         <v>6</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -1043,28 +1063,28 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G15">
         <v>6</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -1072,28 +1092,28 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1">
         <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G16">
         <v>6</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -1101,28 +1121,28 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G17">
         <v>6</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I17">
         <v>2</v>
@@ -1130,28 +1150,28 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>2</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G18">
         <v>6</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I18">
         <v>2</v>
@@ -1159,28 +1179,28 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G19">
         <v>6</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I19">
         <v>2</v>
@@ -1188,7 +1208,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="1">
         <v>2</v>
@@ -1197,19 +1217,19 @@
         <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G20">
         <v>6</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I20">
         <v>2</v>
@@ -1217,7 +1237,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -1226,19 +1246,19 @@
         <v>8</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G21">
         <v>6</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I21">
         <v>2</v>
@@ -1246,7 +1266,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="1">
         <v>3</v>
@@ -1255,19 +1275,19 @@
         <v>9</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G22">
         <v>6</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -1275,28 +1295,28 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1">
         <v>3</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G23">
         <v>6</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -1304,28 +1324,28 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1">
         <v>3</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="G24">
         <v>6</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -1333,28 +1353,28 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" s="1">
         <v>3</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="G25">
         <v>6</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -1362,7 +1382,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="1">
         <v>3</v>
@@ -1371,19 +1391,19 @@
         <v>9</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G26">
         <v>6</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="I26">
         <v>1</v>
@@ -1391,28 +1411,28 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="1">
         <v>3</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="G27">
         <v>6</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I27">
         <v>2</v>
@@ -1420,28 +1440,28 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" s="1">
         <v>3</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G28">
         <v>6</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="I28">
         <v>2</v>
@@ -1449,28 +1469,28 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" s="1">
         <v>3</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G29">
         <v>6</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I29">
         <v>2</v>
@@ -1478,7 +1498,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30" s="1">
         <v>3</v>
@@ -1487,19 +1507,19 @@
         <v>9</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G30">
         <v>6</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I30">
         <v>2</v>
@@ -1507,28 +1527,28 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" s="1">
         <v>3</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G31">
         <v>6</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="I31">
         <v>2</v>
@@ -1536,7 +1556,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32" s="1">
         <v>4</v>
@@ -1545,222 +1565,223 @@
         <v>9</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G32">
         <v>6</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B33" s="1">
         <v>4</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G33">
         <v>6</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="I33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B34" s="1">
         <v>4</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G34">
         <v>6</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="I34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L34" s="3"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B35" s="1">
         <v>4</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G35">
         <v>6</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="I35">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B36" s="1">
         <v>4</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G36">
         <v>6</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="I36">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B37" s="1">
         <v>4</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G37">
         <v>6</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="I37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B38" s="1">
         <v>4</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G38">
         <v>12</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I38">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B39" s="1">
         <v>4</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G39">
         <v>12</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I39">
         <v>2</v>

</xml_diff>

<commit_message>
Optimized the choose year function
</commit_message>
<xml_diff>
--- a/src/dataset.xlsx
+++ b/src/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emili\OneDrive\Escritorio\Universidad\4Carrera\AcademicData\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C1C150-0D81-4C43-8C2D-283DE415592C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31D1C91-09AB-4A36-8A28-BDDD23F94AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82361F5A-4340-435D-A49C-2C3E84564897}"/>
   </bookViews>
@@ -164,9 +164,6 @@
     <t>Databases Admin.</t>
   </si>
   <si>
-    <t>Critic Software</t>
-  </si>
-  <si>
     <t>Algoritmia</t>
   </si>
   <si>
@@ -255,6 +252,9 @@
   </si>
   <si>
     <t>Optative (Internship)</t>
+  </si>
+  <si>
+    <t>Critical Software</t>
   </si>
 </sst>
 </file>
@@ -644,7 +644,7 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -657,7 +657,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -672,16 +672,16 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -707,7 +707,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -715,7 +715,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -724,19 +724,19 @@
         <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3">
-        <v>6</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -753,19 +753,19 @@
         <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4">
-        <v>6</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -794,7 +794,7 @@
         <v>6</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -823,7 +823,7 @@
         <v>6</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -852,7 +852,7 @@
         <v>6</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I7">
         <v>2</v>
@@ -881,7 +881,7 @@
         <v>6</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -910,7 +910,7 @@
         <v>6</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I9">
         <v>2</v>
@@ -939,7 +939,7 @@
         <v>6</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I10">
         <v>2</v>
@@ -968,7 +968,7 @@
         <v>6</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I11">
         <v>2</v>
@@ -997,7 +997,7 @@
         <v>6</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -1026,7 +1026,7 @@
         <v>6</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -1055,7 +1055,7 @@
         <v>6</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -1084,7 +1084,7 @@
         <v>6</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -1113,7 +1113,7 @@
         <v>6</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -1142,7 +1142,7 @@
         <v>6</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I17">
         <v>2</v>
@@ -1171,7 +1171,7 @@
         <v>6</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I18">
         <v>2</v>
@@ -1200,7 +1200,7 @@
         <v>6</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I19">
         <v>2</v>
@@ -1217,7 +1217,7 @@
         <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>24</v>
@@ -1229,7 +1229,7 @@
         <v>6</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I20">
         <v>2</v>
@@ -1258,7 +1258,7 @@
         <v>6</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I21">
         <v>2</v>
@@ -1287,7 +1287,7 @@
         <v>6</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -1301,7 +1301,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>12</v>
@@ -1316,7 +1316,7 @@
         <v>6</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -1330,7 +1330,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>13</v>
@@ -1345,7 +1345,7 @@
         <v>6</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -1374,7 +1374,7 @@
         <v>6</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -1382,7 +1382,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="B26" s="1">
         <v>3</v>
@@ -1403,7 +1403,7 @@
         <v>6</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I26">
         <v>1</v>
@@ -1417,7 +1417,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>13</v>
@@ -1432,7 +1432,7 @@
         <v>6</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I27">
         <v>2</v>
@@ -1440,13 +1440,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" s="1">
         <v>3</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>12</v>
@@ -1461,7 +1461,7 @@
         <v>6</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I28">
         <v>2</v>
@@ -1469,16 +1469,16 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" s="1">
         <v>3</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>24</v>
@@ -1490,7 +1490,7 @@
         <v>6</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I29">
         <v>2</v>
@@ -1498,7 +1498,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="1">
         <v>3</v>
@@ -1519,7 +1519,7 @@
         <v>6</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I30">
         <v>2</v>
@@ -1527,13 +1527,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" s="1">
         <v>3</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>15</v>
@@ -1548,7 +1548,7 @@
         <v>6</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I31">
         <v>2</v>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" s="1">
         <v>4</v>
@@ -1577,7 +1577,7 @@
         <v>6</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I32">
         <v>2</v>
@@ -1585,28 +1585,28 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33" s="1">
         <v>4</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G33">
         <v>6</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I33">
         <v>1</v>
@@ -1614,28 +1614,28 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B34" s="1">
         <v>4</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G34">
         <v>6</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I34">
         <v>1</v>
@@ -1644,28 +1644,28 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B35" s="1">
         <v>4</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G35">
         <v>6</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I35">
         <v>1</v>
@@ -1673,28 +1673,28 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B36" s="1">
         <v>4</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G36">
         <v>6</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I36">
         <v>1</v>
@@ -1702,28 +1702,28 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B37" s="1">
         <v>4</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G37">
         <v>6</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I37">
         <v>1</v>
@@ -1731,28 +1731,28 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B38" s="1">
         <v>4</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G38">
         <v>12</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I38">
         <v>2</v>
@@ -1760,28 +1760,28 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B39" s="1">
         <v>4</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G39">
         <v>12</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I39">
         <v>2</v>

</xml_diff>

<commit_message>
Study of the denomination of the credits
</commit_message>
<xml_diff>
--- a/src/dataset.xlsx
+++ b/src/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emili\OneDrive\Escritorio\Universidad\4Carrera\AcademicData\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31D1C91-09AB-4A36-8A28-BDDD23F94AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586541DF-11BC-4329-AF4B-CF6E3EE96BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82361F5A-4340-435D-A49C-2C3E84564897}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{82361F5A-4340-435D-A49C-2C3E84564897}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="76">
   <si>
     <t>Year</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Algorithms</t>
   </si>
   <si>
-    <t>MH</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -255,6 +252,18 @@
   </si>
   <si>
     <t>Critical Software</t>
+  </si>
+  <si>
+    <t>Denomination</t>
+  </si>
+  <si>
+    <t>Notable</t>
+  </si>
+  <si>
+    <t>Outstanding</t>
+  </si>
+  <si>
+    <t>Honors</t>
   </si>
 </sst>
 </file>
@@ -641,23 +650,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B16DEB-C3AC-4914-94E8-AA9D57CD36CC}">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -669,19 +678,19 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -698,16 +707,16 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2">
         <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -715,7 +724,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -724,19 +733,19 @@
         <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3">
-        <v>6</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -753,19 +762,19 @@
         <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4">
-        <v>6</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -785,16 +794,16 @@
         <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5">
         <v>6</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -814,16 +823,16 @@
         <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6">
         <v>6</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -843,16 +852,16 @@
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7">
         <v>6</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I7">
         <v>2</v>
@@ -872,16 +881,16 @@
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G8">
         <v>6</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -901,16 +910,16 @@
         <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9">
         <v>6</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I9">
         <v>2</v>
@@ -930,16 +939,16 @@
         <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G10">
         <v>6</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I10">
         <v>2</v>
@@ -959,16 +968,16 @@
         <v>15</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11">
         <v>6</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I11">
         <v>2</v>
@@ -988,16 +997,16 @@
         <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12">
         <v>6</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -1005,28 +1014,28 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1">
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G13">
         <v>6</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -1034,7 +1043,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1">
         <v>2</v>
@@ -1046,16 +1055,16 @@
         <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G14">
         <v>6</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -1063,7 +1072,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
@@ -1075,16 +1084,16 @@
         <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G15">
         <v>6</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -1092,7 +1101,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1">
         <v>2</v>
@@ -1104,16 +1113,16 @@
         <v>12</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16">
         <v>6</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -1121,28 +1130,28 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G17">
         <v>6</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I17">
         <v>2</v>
@@ -1150,7 +1159,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1">
         <v>2</v>
@@ -1162,16 +1171,16 @@
         <v>13</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G18">
         <v>6</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I18">
         <v>2</v>
@@ -1179,7 +1188,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
@@ -1191,16 +1200,16 @@
         <v>15</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G19">
         <v>6</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I19">
         <v>2</v>
@@ -1208,7 +1217,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1">
         <v>2</v>
@@ -1217,19 +1226,19 @@
         <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G20">
         <v>6</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I20">
         <v>2</v>
@@ -1237,7 +1246,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -1249,16 +1258,16 @@
         <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G21">
         <v>6</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I21">
         <v>2</v>
@@ -1266,7 +1275,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1">
         <v>3</v>
@@ -1278,16 +1287,16 @@
         <v>13</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G22">
         <v>6</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -1295,28 +1304,28 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="1">
         <v>3</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G23">
         <v>6</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -1324,28 +1333,28 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" s="1">
         <v>3</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="G24">
         <v>6</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -1353,7 +1362,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1">
         <v>3</v>
@@ -1362,19 +1371,19 @@
         <v>17</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="G25">
         <v>6</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -1382,7 +1391,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B26" s="1">
         <v>3</v>
@@ -1394,16 +1403,16 @@
         <v>13</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G26">
         <v>6</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I26">
         <v>1</v>
@@ -1411,28 +1420,28 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="1">
         <v>3</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="G27">
         <v>6</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I27">
         <v>2</v>
@@ -1440,28 +1449,28 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="1">
         <v>3</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G28">
         <v>6</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I28">
         <v>2</v>
@@ -1469,28 +1478,28 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="1">
         <v>3</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G29">
         <v>6</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I29">
         <v>2</v>
@@ -1498,7 +1507,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" s="1">
         <v>3</v>
@@ -1510,16 +1519,16 @@
         <v>13</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G30">
         <v>6</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I30">
         <v>2</v>
@@ -1527,28 +1536,28 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="1">
         <v>3</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G31">
         <v>6</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I31">
         <v>2</v>
@@ -1556,7 +1565,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32" s="1">
         <v>4</v>
@@ -1568,16 +1577,16 @@
         <v>14</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G32">
         <v>6</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I32">
         <v>2</v>
@@ -1585,28 +1594,28 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33" s="1">
         <v>4</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G33">
         <v>6</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I33">
         <v>1</v>
@@ -1614,28 +1623,28 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34" s="1">
         <v>4</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G34">
         <v>6</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I34">
         <v>1</v>
@@ -1644,28 +1653,28 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B35" s="1">
         <v>4</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G35">
         <v>6</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I35">
         <v>1</v>
@@ -1673,28 +1682,28 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B36" s="1">
         <v>4</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G36">
         <v>6</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I36">
         <v>1</v>
@@ -1702,28 +1711,28 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B37" s="1">
         <v>4</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G37">
         <v>6</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I37">
         <v>1</v>
@@ -1731,28 +1740,28 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B38" s="1">
         <v>4</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G38">
         <v>12</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I38">
         <v>2</v>
@@ -1760,32 +1769,35 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" s="1">
         <v>4</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G39">
         <v>12</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I39">
         <v>2</v>
       </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G46" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>